<commit_message>
added credit voucher functionality for ABO
</commit_message>
<xml_diff>
--- a/na-amway-qa-api-automation-cart-backend-master/src/main/resources/testdata/data/AamwayAPIData.xlsx
+++ b/na-amway-qa-api-automation-cart-backend-master/src/main/resources/testdata/data/AamwayAPIData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="createpayment" sheetId="1" state="visible" r:id="rId3"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="28">
   <si>
     <t xml:space="preserve">testCaseName</t>
   </si>
@@ -97,9 +97,6 @@
   </si>
   <si>
     <t xml:space="preserve">tcAmwayAPICreditVoucherCreatePayment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kul-01222</t>
   </si>
   <si>
     <t xml:space="preserve">100</t>
@@ -485,7 +482,7 @@
   </sheetPr>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
     </sheetView>
   </sheetViews>
@@ -571,17 +568,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.4765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.4765625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="42.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="34.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="42.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="23.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="34.49"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -589,30 +587,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J1" s="1" t="s">
         <v>17</v>
       </c>
     </row>
@@ -621,13 +616,13 @@
         <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>26</v>
@@ -635,16 +630,13 @@
       <c r="F2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="4" t="n">
+      <c r="H2" s="4" t="n">
         <v>694806621</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added code for UI Automation
</commit_message>
<xml_diff>
--- a/na-amway-qa-api-automation-cart-backend-master/src/main/resources/testdata/data/AamwayAPIData.xlsx
+++ b/na-amway-qa-api-automation-cart-backend-master/src/main/resources/testdata/data/AamwayAPIData.xlsx
@@ -5,12 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="createpayment" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="creditcardcreatepayment" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="ampursecreatePayment" sheetId="2" state="visible" r:id="rId4"/>
     <sheet name="creditvouchercreatepayment" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="ampointscreatepayment" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="payatshopcreatepayment" sheetId="5" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,14 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="31">
   <si>
     <t xml:space="preserve">testCaseName</t>
   </si>
   <si>
-    <t xml:space="preserve">rfid</t>
-  </si>
-  <si>
     <t xml:space="preserve">refType</t>
   </si>
   <si>
@@ -48,10 +47,13 @@
     <t xml:space="preserve">entryType</t>
   </si>
   <si>
-    <t xml:space="preserve">tcAmwayAPICreatePayment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kul-0019</t>
+    <t xml:space="preserve">accountId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">profileId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tcAmwayAPICreditCardCreatePayment</t>
   </si>
   <si>
     <t xml:space="preserve">ORDER</t>
@@ -60,7 +62,7 @@
     <t xml:space="preserve">THB</t>
   </si>
   <si>
-    <t xml:space="preserve">1400</t>
+    <t xml:space="preserve">100</t>
   </si>
   <si>
     <t xml:space="preserve">990ee4a8-7f8c-4cb6-b4c1-957500861f8e</t>
@@ -72,10 +74,7 @@
     <t xml:space="preserve">INITIATE</t>
   </si>
   <si>
-    <t xml:space="preserve">accountId</t>
-  </si>
-  <si>
-    <t xml:space="preserve">profileId</t>
+    <t xml:space="preserve">8e4260f0-9f5f-4b31-ae54-2a46d118ca0c</t>
   </si>
   <si>
     <t xml:space="preserve">tcAmwayAPIAmpurseCreatePayment</t>
@@ -90,22 +89,34 @@
     <t xml:space="preserve">AB_AMPURSE</t>
   </si>
   <si>
-    <t xml:space="preserve">AUTH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8e4260f0-9f5f-4b31-ae54-2a46d118ca0c</t>
+    <t xml:space="preserve">CAPTURE</t>
   </si>
   <si>
     <t xml:space="preserve">tcAmwayAPICreditVoucherCreatePayment</t>
   </si>
   <si>
-    <t xml:space="preserve">100</t>
-  </si>
-  <si>
     <t xml:space="preserve">9b4ded64-be70-42f7-b648-ba08c88b3f15</t>
   </si>
   <si>
     <t xml:space="preserve">AB_CREDIT_VOUCHER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tcAmwayAPIAmpointsCreatePayment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">815bbc07-38aa-4abb-a2a5-383d7277d123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AMPOINTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tcAmwayAPIPayatShopCreatePayment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9eaf9830-6f0f-4c73-9121-d4e29f9a252d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BILLPAY_QR_CODE</t>
   </si>
 </sst>
 </file>
@@ -116,7 +127,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,11 +155,17 @@
       <color rgb="FF000000"/>
       <name val="Courier New"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF2A00FF"/>
+      <name val="Courier New"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF2A00FF"/>
+      <color rgb="FF000000"/>
       <name val="Courier New"/>
       <family val="0"/>
       <charset val="1"/>
@@ -196,7 +213,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -214,6 +231,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -400,16 +421,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.4765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.4765625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="42.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="33.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="42.65"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -431,37 +452,43 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>15</v>
+      </c>
+      <c r="H2" s="4" t="n">
+        <v>694806621</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -483,7 +510,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.4765625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -499,33 +526,33 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>10</v>
@@ -534,22 +561,22 @@
         <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="H2" s="4" t="n">
         <v>694806621</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -570,15 +597,15 @@
   </sheetPr>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.4765625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="42.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="23.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="23.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="34.49"/>
   </cols>
   <sheetData>
@@ -587,33 +614,33 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>24</v>
+      <c r="A2" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>10</v>
@@ -622,7 +649,95 @@
         <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="4" t="n">
+        <v>694806621</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="13.4765625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="47.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="42.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="23.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="34.49"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
         <v>25</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>26</v>
@@ -631,13 +746,102 @@
         <v>27</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="H2" s="4" t="n">
+        <v>231494708</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I25" activeCellId="0" sqref="I25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="13.4765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="35.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="34.49"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="H2" s="4" t="n">
         <v>694806621</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit code for ABO
</commit_message>
<xml_diff>
--- a/na-amway-qa-api-automation-cart-backend-master/src/main/resources/testdata/data/AamwayAPIData.xlsx
+++ b/na-amway-qa-api-automation-cart-backend-master/src/main/resources/testdata/data/AamwayAPIData.xlsx
@@ -5,14 +5,16 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="creditcardcreatepayment" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="ampursecreatePayment" sheetId="2" state="visible" r:id="rId4"/>
-    <sheet name="creditvouchercreatepayment" sheetId="3" state="visible" r:id="rId5"/>
-    <sheet name="ampointscreatepayment" sheetId="4" state="visible" r:id="rId6"/>
-    <sheet name="payatshopcreatepayment" sheetId="5" state="visible" r:id="rId7"/>
+    <sheet name="onlinebanktransfercreatepayment" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="splitampurseobtcreatepayment" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="ampursecreatePayment" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="creditvouchercreatepayment" sheetId="5" state="visible" r:id="rId7"/>
+    <sheet name="ampointscreatepayment" sheetId="6" state="visible" r:id="rId8"/>
+    <sheet name="payatshopcreatepayment" sheetId="7" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="44">
   <si>
     <t xml:space="preserve">testCaseName</t>
   </si>
@@ -77,19 +79,58 @@
     <t xml:space="preserve">8e4260f0-9f5f-4b31-ae54-2a46d118ca0c</t>
   </si>
   <si>
+    <t xml:space="preserve">tcAmwayAPIOnlineBankTransferCreatePayment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">223f6522-3f8e-41ce-8ad7-192319481873</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ONLINE_BANK_TRANSFER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">totalAmount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">obtPaymentMethodProviderId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">obtPaymentMethodCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">obtEntryType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">obtAmount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ampursePaymentMethodProviderId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ampursePaymentMethodCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ampurseEntryType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ampurseAmount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tcAmwayAPISplitAmpurseOBTCreatePayment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a301ee43-8969-4bb5-8353-8024bebc153a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AB_AMPURSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAPTURE</t>
+  </si>
+  <si>
     <t xml:space="preserve">tcAmwayAPIAmpurseCreatePayment</t>
   </si>
   <si>
     <t xml:space="preserve">4500</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a301ee43-8969-4bb5-8353-8024bebc153a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AB_AMPURSE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAPTURE</t>
   </si>
   <si>
     <t xml:space="preserve">tcAmwayAPICreditVoucherCreatePayment</t>
@@ -127,7 +168,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -155,17 +196,11 @@
       <color rgb="FF000000"/>
       <name val="Courier New"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF2A00FF"/>
-      <name val="Courier New"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Courier New"/>
       <family val="0"/>
       <charset val="1"/>
@@ -213,7 +248,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -231,10 +266,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -423,7 +454,7 @@
   </sheetPr>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -503,6 +534,214 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="13.4765625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="54.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="42.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="21.03"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="4" t="n">
+        <v>694806621</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="13.4765625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="54.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="42.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="21.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="10.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="42.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="25.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="16.49"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="4" t="n">
+        <v>694806621</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" s="1" t="n">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -551,8 +790,8 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>17</v>
+      <c r="A2" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>10</v>
@@ -561,16 +800,16 @@
         <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="H2" s="4" t="n">
         <v>694806621</v>
@@ -590,7 +829,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -639,8 +878,8 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>22</v>
+      <c r="A2" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>10</v>
@@ -652,13 +891,13 @@
         <v>12</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="H2" s="4" t="n">
         <v>694806621</v>
@@ -678,7 +917,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -727,8 +966,8 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>25</v>
+      <c r="A2" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>10</v>
@@ -740,13 +979,13 @@
         <v>12</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="H2" s="4" t="n">
         <v>231494708</v>
@@ -766,7 +1005,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -774,7 +1013,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I25" activeCellId="0" sqref="I25"/>
+      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.4765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -816,8 +1055,8 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>28</v>
+      <c r="A2" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>10</v>
@@ -829,10 +1068,10 @@
         <v>12</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
commit for abo and member
</commit_message>
<xml_diff>
--- a/na-amway-qa-api-automation-cart-backend-master/src/main/resources/testdata/data/AamwayAPIData.xlsx
+++ b/na-amway-qa-api-automation-cart-backend-master/src/main/resources/testdata/data/AamwayAPIData.xlsx
@@ -168,7 +168,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,6 +204,12 @@
       <name val="Courier New"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF2AA198"/>
+      <name val="Courier New"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -248,7 +254,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -266,6 +272,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -329,7 +339,7 @@
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF2AA198"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
@@ -627,8 +637,8 @@
   </sheetPr>
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.4765625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -687,7 +697,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="5" t="s">
         <v>29</v>
       </c>
       <c r="B2" s="2" t="s">

</xml_diff>